<commit_message>
Update Nalco PDF (2025-11-19 06:49:24 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>292.65</v>
+        <v>281.95</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>297.15</v>
+        <v>292.65</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,42 +920,70 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C18" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E18" s="3" t="inlineStr">
+      <c r="E19" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F18" s="3" t="inlineStr">
+      <c r="F19" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -980,6 +1008,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F16" r:id="rId15"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F17" r:id="rId16"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F18" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F19" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-11-22 03:48:57 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>281.95</v>
+        <v>283.55</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>292.65</v>
+        <v>281.95</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>297.15</v>
+        <v>292.65</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,22 +920,22 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
@@ -948,42 +948,70 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E19" s="3" t="inlineStr">
+      <c r="E20" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F19" s="3" t="inlineStr">
+      <c r="F20" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -1009,6 +1037,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F17" r:id="rId16"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F18" r:id="rId17"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F19" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-11-27 06:52:13 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>283.55</v>
+        <v>290.95</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>281.95</v>
+        <v>283.55</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>292.65</v>
+        <v>281.95</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>297.15</v>
+        <v>292.65</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,22 +920,22 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
@@ -948,22 +948,22 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
@@ -976,42 +976,70 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B20" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E20" s="3" t="inlineStr">
+      <c r="E21" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F20" s="3" t="inlineStr">
+      <c r="F21" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -1038,6 +1066,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F18" r:id="rId17"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F19" r:id="rId18"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F20" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-12-02 06:53:25 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -599,7 +599,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,22 +920,22 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
@@ -948,22 +948,22 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
@@ -976,22 +976,22 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
@@ -1004,42 +1004,70 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B21" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C21" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E21" s="3" t="inlineStr">
+      <c r="E22" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F21" s="3" t="inlineStr">
+      <c r="F22" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -1067,6 +1095,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F19" r:id="rId18"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F20" r:id="rId19"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F21" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-12-05 09:41:15 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>290.95</v>
+        <v>296.05</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>283.55</v>
+        <v>290.95</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>281.95</v>
+        <v>283.55</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>292.65</v>
+        <v>281.95</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>296.05</v>
+        <v>292.65</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,22 +920,22 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
@@ -948,22 +948,22 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
@@ -976,22 +976,22 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
@@ -1004,22 +1004,22 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
@@ -1032,42 +1032,70 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B22" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="n">
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E22" s="3" t="inlineStr">
+      <c r="E23" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F22" s="3" t="inlineStr">
+      <c r="F23" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -1096,6 +1124,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F20" r:id="rId19"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F21" r:id="rId20"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F23" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-12-24 06:55:04 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>296.05</v>
+        <v>301.65</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>24-12-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-24-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>290.95</v>
+        <v>296.05</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>283.55</v>
+        <v>290.95</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>281.95</v>
+        <v>283.55</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>292.65</v>
+        <v>281.95</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>296.05</v>
+        <v>292.65</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,22 +920,22 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
@@ -948,22 +948,22 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
@@ -976,22 +976,22 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
@@ -1004,22 +1004,22 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
@@ -1032,22 +1032,22 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
@@ -1060,42 +1060,70 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B23" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C23" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D23" s="4" t="n">
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E23" s="3" t="inlineStr">
+      <c r="E24" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F23" s="3" t="inlineStr">
+      <c r="F24" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -1125,6 +1153,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F21" r:id="rId20"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId21"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F23" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F24" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2026-01-02 06:54:49 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>301.65</v>
+        <v>307.25</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>24-12-2025</t>
+          <t>01-01-2026</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-24-12-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-01-2026.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>296.05</v>
+        <v>301.65</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>24-12-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-24-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>290.95</v>
+        <v>296.05</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>283.55</v>
+        <v>290.95</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>281.95</v>
+        <v>283.55</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>292.65</v>
+        <v>281.95</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>296.05</v>
+        <v>292.65</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,22 +920,22 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
@@ -948,22 +948,22 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
@@ -976,22 +976,22 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
@@ -1004,22 +1004,22 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
@@ -1032,22 +1032,22 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
@@ -1060,22 +1060,22 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
@@ -1088,42 +1088,70 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B24" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C24" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D24" s="4" t="n">
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D25" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E24" s="3" t="inlineStr">
+      <c r="E25" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F24" s="3" t="inlineStr">
+      <c r="F25" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -1154,6 +1182,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId21"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F23" r:id="rId22"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F24" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F25" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2026-01-07 06:55:58 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>307.25</v>
+        <v>320.05</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>01-01-2026</t>
+          <t>07-01-2026</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-01-2026.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2026/01/Ingot-07-01-2026.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>301.65</v>
+        <v>307.25</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>24-12-2025</t>
+          <t>01-01-2026</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-24-12-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-01-2026.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>296.05</v>
+        <v>301.65</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>24-12-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-24-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>290.95</v>
+        <v>296.05</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>283.55</v>
+        <v>290.95</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>281.95</v>
+        <v>283.55</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>292.65</v>
+        <v>281.95</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>296.05</v>
+        <v>292.65</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,22 +920,22 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
@@ -948,22 +948,22 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
@@ -976,22 +976,22 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
@@ -1004,22 +1004,22 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
@@ -1032,22 +1032,22 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
@@ -1060,22 +1060,22 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
@@ -1088,22 +1088,22 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
@@ -1116,42 +1116,70 @@
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B25" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C25" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D25" s="4" t="n">
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E25" s="3" t="inlineStr">
+      <c r="E26" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F25" s="3" t="inlineStr">
+      <c r="F26" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -1183,6 +1211,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F23" r:id="rId22"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F24" r:id="rId23"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F25" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F26" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2026-01-14 06:55:57 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>320.05</v>
+        <v>330.75</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>07-01-2026</t>
+          <t>14-01-2026</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2026/01/Ingot-07-01-2026.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-01-2026.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>307.25</v>
+        <v>320.05</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>01-01-2026</t>
+          <t>07-01-2026</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-01-2026.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2026/01/Ingot-07-01-2026.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>301.65</v>
+        <v>307.25</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>24-12-2025</t>
+          <t>01-01-2026</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-24-12-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-01-2026.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>296.05</v>
+        <v>301.65</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>24-12-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-24-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>290.95</v>
+        <v>296.05</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-05-12-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>283.55</v>
+        <v>290.95</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-27-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>281.95</v>
+        <v>283.55</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/11/Ingot-22-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>292.65</v>
+        <v>281.95</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-19-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>296.05</v>
+        <v>292.65</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
@@ -920,22 +920,22 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
@@ -948,22 +948,22 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
@@ -976,22 +976,22 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
@@ -1004,22 +1004,22 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
@@ -1032,22 +1032,22 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
@@ -1060,22 +1060,22 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
@@ -1088,22 +1088,22 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
@@ -1116,22 +1116,22 @@
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
@@ -1144,42 +1144,70 @@
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F26" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B26" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C26" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D26" s="4" t="n">
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D27" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E26" s="3" t="inlineStr">
+      <c r="E27" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F26" s="3" t="inlineStr">
+      <c r="F27" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -1212,6 +1240,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F24" r:id="rId23"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F25" r:id="rId24"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F26" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F27" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>